<commit_message>
some metadata updates from Kiki
</commit_message>
<xml_diff>
--- a/tabular/3. BTV DB all segs 2016-12-31_data_missing.xlsx
+++ b/tabular/3. BTV DB all segs 2016-12-31_data_missing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4640" yWindow="3600" windowWidth="39440" windowHeight="19300" tabRatio="500"/>
+    <workbookView xWindow="380" yWindow="4020" windowWidth="25640" windowHeight="19300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="query_result.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8574" uniqueCount="5201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8585" uniqueCount="5201">
   <si>
     <t>sequence_id</t>
   </si>
@@ -19336,8 +19336,8 @@
   <dimension ref="A1:K4925"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4823" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4827" sqref="C4827"/>
+      <pane ySplit="1" topLeftCell="A2847" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2865" sqref="E2865"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -25208,7 +25208,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="625" spans="1:4">
+    <row r="625" spans="1:8">
       <c r="A625" s="2" t="s">
         <v>662</v>
       </c>
@@ -25219,7 +25219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="626" spans="1:4">
+    <row r="626" spans="1:8">
       <c r="A626" s="2" t="s">
         <v>663</v>
       </c>
@@ -25227,7 +25227,7 @@
         <v>4623</v>
       </c>
     </row>
-    <row r="627" spans="1:4">
+    <row r="627" spans="1:8">
       <c r="A627" s="2" t="s">
         <v>664</v>
       </c>
@@ -25238,7 +25238,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="628" spans="1:4">
+    <row r="628" spans="1:8">
       <c r="A628" s="2" t="s">
         <v>665</v>
       </c>
@@ -25249,7 +25249,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="629" spans="1:4">
+    <row r="629" spans="1:8">
       <c r="A629" s="2" t="s">
         <v>666</v>
       </c>
@@ -25260,7 +25260,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="630" spans="1:4">
+    <row r="630" spans="1:8">
       <c r="A630" s="2" t="s">
         <v>667</v>
       </c>
@@ -25268,7 +25268,7 @@
         <v>4627</v>
       </c>
     </row>
-    <row r="631" spans="1:4">
+    <row r="631" spans="1:8">
       <c r="A631" s="2" t="s">
         <v>668</v>
       </c>
@@ -25276,7 +25276,7 @@
         <v>4628</v>
       </c>
     </row>
-    <row r="632" spans="1:4">
+    <row r="632" spans="1:8">
       <c r="A632" s="2" t="s">
         <v>669</v>
       </c>
@@ -25287,7 +25287,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="633" spans="1:4">
+    <row r="633" spans="1:8">
       <c r="A633" s="2" t="s">
         <v>670</v>
       </c>
@@ -25295,7 +25295,7 @@
         <v>4620</v>
       </c>
     </row>
-    <row r="634" spans="1:4">
+    <row r="634" spans="1:8">
       <c r="A634" s="2" t="s">
         <v>671</v>
       </c>
@@ -25303,23 +25303,35 @@
         <v>4630</v>
       </c>
     </row>
-    <row r="635" spans="1:4">
+    <row r="635" spans="1:8">
       <c r="A635" s="2" t="s">
         <v>672</v>
       </c>
       <c r="C635" s="1" t="s">
         <v>4631</v>
       </c>
-    </row>
-    <row r="636" spans="1:4">
+      <c r="G635" s="9" t="s">
+        <v>1736</v>
+      </c>
+      <c r="H635" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="636" spans="1:8">
       <c r="A636" s="2" t="s">
         <v>673</v>
       </c>
       <c r="C636" s="1" t="s">
         <v>4632</v>
       </c>
-    </row>
-    <row r="637" spans="1:4">
+      <c r="G636" s="9" t="s">
+        <v>1673</v>
+      </c>
+      <c r="H636" s="9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="637" spans="1:8">
       <c r="A637" s="2" t="s">
         <v>674</v>
       </c>
@@ -25330,7 +25342,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="638" spans="1:4">
+    <row r="638" spans="1:8">
       <c r="A638" s="2" t="s">
         <v>675</v>
       </c>
@@ -25341,7 +25353,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="639" spans="1:4">
+    <row r="639" spans="1:8">
       <c r="A639" s="2" t="s">
         <v>676</v>
       </c>
@@ -25352,7 +25364,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="640" spans="1:4">
+    <row r="640" spans="1:8">
       <c r="A640" s="2" t="s">
         <v>677</v>
       </c>
@@ -47869,6 +47881,9 @@
       <c r="A2846" s="2" t="s">
         <v>2937</v>
       </c>
+      <c r="C2846" s="9" t="s">
+        <v>4759</v>
+      </c>
     </row>
     <row r="2847" spans="1:3">
       <c r="A2847" s="2" t="s">
@@ -47882,6 +47897,9 @@
       <c r="A2848" s="2" t="s">
         <v>2939</v>
       </c>
+      <c r="C2848" s="9" t="s">
+        <v>4759</v>
+      </c>
     </row>
     <row r="2849" spans="1:3">
       <c r="A2849" s="2" t="s">
@@ -47911,6 +47929,9 @@
       <c r="A2852" s="2" t="s">
         <v>2943</v>
       </c>
+      <c r="C2852" s="9" t="s">
+        <v>4759</v>
+      </c>
     </row>
     <row r="2853" spans="1:3">
       <c r="A2853" s="2" t="s">
@@ -47932,26 +47953,41 @@
       <c r="A2855" s="2" t="s">
         <v>2946</v>
       </c>
+      <c r="C2855" s="9" t="s">
+        <v>4759</v>
+      </c>
     </row>
     <row r="2856" spans="1:3">
       <c r="A2856" s="2" t="s">
         <v>2947</v>
       </c>
+      <c r="C2856" s="9" t="s">
+        <v>4759</v>
+      </c>
     </row>
     <row r="2857" spans="1:3">
       <c r="A2857" s="2" t="s">
         <v>2948</v>
       </c>
+      <c r="C2857" s="9" t="s">
+        <v>4759</v>
+      </c>
     </row>
     <row r="2858" spans="1:3">
       <c r="A2858" s="2" t="s">
         <v>2949</v>
       </c>
+      <c r="C2858" s="9" t="s">
+        <v>4759</v>
+      </c>
     </row>
     <row r="2859" spans="1:3">
       <c r="A2859" s="2" t="s">
         <v>2950</v>
       </c>
+      <c r="C2859" s="9" t="s">
+        <v>4759</v>
+      </c>
     </row>
     <row r="2860" spans="1:3">
       <c r="A2860" s="2" t="s">
@@ -47980,6 +48016,9 @@
     <row r="2863" spans="1:3">
       <c r="A2863" s="2" t="s">
         <v>2954</v>
+      </c>
+      <c r="C2863" s="9" t="s">
+        <v>4759</v>
       </c>
     </row>
     <row r="2864" spans="1:3">

</xml_diff>

<commit_message>
glue version update, tabular update and check segments script based on blast recogniser.
</commit_message>
<xml_diff>
--- a/tabular/3. BTV DB all segs 2016-12-31_data_missing.xlsx
+++ b/tabular/3. BTV DB all segs 2016-12-31_data_missing.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8585" uniqueCount="5198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8585" uniqueCount="5197">
   <si>
     <t>sequence_id</t>
   </si>
@@ -15607,9 +15607,6 @@
   </si>
   <si>
     <t>Serbia</t>
-  </si>
-  <si>
-    <t>Bosnia</t>
   </si>
   <si>
     <t>Trinidad and Tobago</t>
@@ -19327,8 +19324,8 @@
   <dimension ref="A1:K4925"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1006" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1021" sqref="A1:I4839"/>
+      <pane ySplit="1" topLeftCell="A4494" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4509" sqref="E4509"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -26385,7 +26382,7 @@
         <v>7</v>
       </c>
       <c r="E700" s="2" t="s">
-        <v>5197</v>
+        <v>5196</v>
       </c>
       <c r="F700" s="2">
         <v>1989</v>
@@ -26470,7 +26467,7 @@
         <v>7</v>
       </c>
       <c r="E705" s="2" t="s">
-        <v>5197</v>
+        <v>5196</v>
       </c>
       <c r="F705" s="2">
         <v>1988</v>
@@ -62918,7 +62915,7 @@
         <v>2</v>
       </c>
       <c r="E4509" s="2" t="s">
-        <v>5196</v>
+        <v>81</v>
       </c>
       <c r="F4509" s="2">
         <v>2002</v>

</xml_diff>